<commit_message>
workflowr is not working
</commit_message>
<xml_diff>
--- a/3_output/reactome_sig.xlsx
+++ b/3_output/reactome_sig.xlsx
@@ -362,48 +362,50 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>GeneRatio</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pvalue</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>p.adjust</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>logFDR</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>qvalue</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>geneID</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Count</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GeneRatio</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>pvalue</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>p.adjust</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>logFDR</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>qvalue</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>geneID</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>56</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Neuronal System</t>
+        </is>
       </c>
       <c r="B2">
         <v>0.1744548286604361</v>
@@ -422,18 +424,18 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Neuronal System</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
           <t>Kcnk3/Kcnb2/Syn2/Slc1a3/Kcnj3/Gria4/Kcna6/Kcnd2/Ptprd/Kcnd3/Nlgn1/Epb41l3/Abat/Lrrc7/Gnai1/Lrrc4b/Kcnq5/Grin2b/Adcy3/Shank2/Maoa/Gngt2/Plcb1/Ppfia2/Slitrk3/Rps6ka2/Glrb/Ppfia4/Adcy4/Adcy7/Gabra4/Dlg2/Gng11/Lin7a/Nlgn3/Tspan7/Kcnma1/Gjc1/Gng2/Kcnc4/Plcb2/Slc38a1/Lrfn2/Dlg4/Kcng4/Gnb5/Arhgef9/Gnb4/Gabbr1/Kcnq4/Cacna1a/Cacnb4/Prkar1b/Kcnh1/Camk1/Nlgn2</t>
         </is>
       </c>
+      <c r="H2">
+        <v>56</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>44</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Extracellular matrix organization</t>
+        </is>
       </c>
       <c r="B3">
         <v>0.1904761904761905</v>
@@ -452,18 +454,18 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Extracellular matrix organization</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
           <t>Col11a1/Mmp16/Col26a1/Itga4/P3h3/Col14a1/Capn6/Ddr2/Col4a6/Cd44/Lama4/Col16a1/Itgb7/Fn1/Mmp2/Icam1/Nid1/Jam3/Itga1/Col13a1/Loxl3/Itgal/Emilin1/Pecam1/Col5a2/Ltbp3/Mmp19/Bgn/Col15a1/P3h1/Adam19/Efemp2/Crtap/Col23a1/Col18a1/Itga8/Itgb4/Tmprss6/Lum/Nid2/Bmp7/Jam2/Fbln5/Col4a5</t>
         </is>
       </c>
+      <c r="H3">
+        <v>44</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4">
-        <v>71</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hemostasis</t>
+        </is>
       </c>
       <c r="B4">
         <v>0.1451942740286299</v>
@@ -482,18 +484,18 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Hemostasis</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
           <t>Apob/Hgf/Angpt1/Itga4/Cd109/Igf1/Tfpi/Slc8a1/Nos3/Cd44/Pcdh7/P2rx2/Gnai1/Fn1/Pde1b/Serpine2/Jam3/Tek/Gngt2/Pik3r6/Dock2/Rasgrp2/Slc8a3/Trpc6/Sh2b2/Kif26a/Dock10/Maged2/Islr/Procr/Gng11/Itgal/Esam/Dgkb/Tubb4a/Vegfc/Pde1a/Sele/Pecam1/Kif6/Igf2/Gng2/Pros1/Arrb1/Sccpdh/Arrb2/Fyn/Pde5a/Cd84/Tor4a/Fgr/Habp4/Atp2b4/Gnb5/Fam3c/Selenop/Gnb4/Apbb1ip/Sri/Lat/Vps45/Kif16b/Spn/Lcp2/Pafah2/Lhfpl2/F2r/Prkar1b/Kif5a/Plek/Jam2</t>
         </is>
       </c>
+      <c r="H4">
+        <v>71</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5">
-        <v>19</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Platelet homeostasis</t>
+        </is>
       </c>
       <c r="B5">
         <v>0.2676056338028169</v>
@@ -512,18 +514,18 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Platelet homeostasis</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
           <t>Apob/Slc8a1/Nos3/P2rx2/Pde1b/Gngt2/Slc8a3/Trpc6/Gng11/Pde1a/Pecam1/Gng2/Pde5a/Fgr/Atp2b4/Gnb5/Gnb4/Sri/Pafah2</t>
         </is>
       </c>
+      <c r="H5">
+        <v>19</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6">
-        <v>18</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Integrin cell surface interactions</t>
+        </is>
       </c>
       <c r="B6">
         <v>0.2727272727272727</v>
@@ -542,18 +544,19 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Integrin cell surface interactions</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
           <t>Itga4/Col4a6/Cd44/Col16a1/Itgb7/Fn1/Icam1/Jam3/Itga1/Col13a1/Itgal/Pecam1/Col5a2/Col18a1/Itga8/Lum/Jam2/Col4a5</t>
         </is>
       </c>
+      <c r="H6">
+        <v>18</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7">
-        <v>35</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Transmission across Chemical
+Synapses</t>
+        </is>
       </c>
       <c r="B7">
         <v>0.1758793969849246</v>
@@ -572,19 +575,19 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Transmission across Chemical
-Synapses</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
           <t>Syn2/Slc1a3/Kcnj3/Gria4/Abat/Lrrc7/Gnai1/Grin2b/Adcy3/Maoa/Gngt2/Plcb1/Ppfia2/Rps6ka2/Glrb/Ppfia4/Adcy4/Adcy7/Gabra4/Dlg2/Gng11/Lin7a/Tspan7/Gng2/Plcb2/Slc38a1/Dlg4/Gnb5/Arhgef9/Gnb4/Gabbr1/Cacna1a/Cacnb4/Prkar1b/Camk1</t>
         </is>
       </c>
+      <c r="H7">
+        <v>35</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8">
-        <v>12</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>O-glycosylation of TSR
+domain-containing proteins</t>
+        </is>
       </c>
       <c r="B8">
         <v>0.3636363636363636</v>
@@ -603,19 +606,18 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>O-glycosylation of TSR
-domain-containing proteins</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
           <t>Adamts20/Sema5b/Adamts16/Adamts19/Thsd7b/Thsd1/Adamts1/Adamts10/Adamts7/Adamtsl1/Sbspon/Adamts17</t>
         </is>
       </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9">
-        <v>21</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>O-linked glycosylation</t>
+        </is>
       </c>
       <c r="B9">
         <v>0.21875</v>
@@ -634,18 +636,19 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>O-linked glycosylation</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
           <t>Adamts20/Sema5b/Adamts16/Adamts19/Thsd7b/Thsd1/Adamts1/Galnt16/St3gal2/St6galnac4/Adamts10/Adamts7/Galntl6/Adamtsl1/Pomt2/Large1/B3gnt5/St3gal4/Sbspon/Adamts17/Galnt18</t>
         </is>
       </c>
+      <c r="H9">
+        <v>21</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10">
-        <v>25</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Neurotransmitter receptors and
+postsynaptic signal transmission</t>
+        </is>
       </c>
       <c r="B10">
         <v>0.1838235294117647</v>
@@ -664,19 +667,18 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Neurotransmitter receptors and
-postsynaptic signal transmission</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
           <t>Kcnj3/Gria4/Lrrc7/Gnai1/Grin2b/Adcy3/Gngt2/Plcb1/Rps6ka2/Glrb/Adcy4/Adcy7/Gabra4/Dlg2/Gng11/Tspan7/Gng2/Plcb2/Dlg4/Gnb5/Arhgef9/Gnb4/Gabbr1/Prkar1b/Camk1</t>
         </is>
       </c>
+      <c r="H10">
+        <v>25</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11">
-        <v>16</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>G alpha (12/13) signalling events</t>
+        </is>
       </c>
       <c r="B11">
         <v>0.2285714285714286</v>
@@ -695,18 +697,18 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>G alpha (12/13) signalling events</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
           <t>Plxnb1/Adra1a/Arhgef25/Gngt2/Gng11/Arhgef15/Gng2/Arhgef26/Net1/Fgd1/Gnb5/Ngef/Arhgef9/Gnb4/Fgd2/Plekhg5</t>
         </is>
       </c>
+      <c r="H11">
+        <v>16</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12">
-        <v>10</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>G alpha (z) signalling events</t>
+        </is>
       </c>
       <c r="B12">
         <v>0.3225806451612903</v>
@@ -725,18 +727,19 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>G alpha (z) signalling events</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
           <t>Rgs16/Adcy3/Gngt2/Adcy4/Adcy7/Gng11/Gng2/Gnaz/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13">
-        <v>15</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Protein-protein interactions at
+synapses</t>
+        </is>
       </c>
       <c r="B13">
         <v>0.2272727272727273</v>
@@ -755,19 +758,19 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Protein-protein interactions at
-synapses</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
           <t>Gria4/Ptprd/Nlgn1/Epb41l3/Lrrc4b/Grin2b/Shank2/Ppfia2/Slitrk3/Ppfia4/Dlg2/Nlgn3/Lrfn2/Dlg4/Nlgn2</t>
         </is>
       </c>
+      <c r="H13">
+        <v>15</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14">
-        <v>14</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Collagen biosynthesis and modifying
+enzymes</t>
+        </is>
       </c>
       <c r="B14">
         <v>0.2333333333333333</v>
@@ -786,19 +789,18 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Collagen biosynthesis and modifying
-enzymes</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
           <t>Col11a1/Col26a1/P3h3/Col14a1/Col4a6/Col16a1/Col13a1/Col5a2/Col15a1/P3h1/Crtap/Col23a1/Col18a1/Col4a5</t>
         </is>
       </c>
+      <c r="H14">
+        <v>14</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15">
-        <v>11</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>GABA B receptor activation</t>
+        </is>
       </c>
       <c r="B15">
         <v>0.275</v>
@@ -817,18 +819,18 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>GABA B receptor activation</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
           <t>Kcnj3/Gnai1/Adcy3/Gngt2/Adcy4/Adcy7/Gng11/Gng2/Gnb5/Gnb4/Gabbr1</t>
         </is>
       </c>
+      <c r="H15">
+        <v>11</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16">
-        <v>11</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Activation of GABAB receptors</t>
+        </is>
       </c>
       <c r="B16">
         <v>0.275</v>
@@ -847,18 +849,19 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Activation of GABAB receptors</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
           <t>Kcnj3/Gnai1/Adcy3/Gngt2/Adcy4/Adcy7/Gng11/Gng2/Gnb5/Gnb4/Gabbr1</t>
         </is>
       </c>
+      <c r="H16">
+        <v>11</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17">
-        <v>35</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Platelet activation, signaling and
+aggregation</t>
+        </is>
       </c>
       <c r="B17">
         <v>0.1440329218106996</v>
@@ -877,19 +880,18 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Platelet activation, signaling and
-aggregation</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
           <t>Hgf/Cd109/Igf1/Pcdh7/Gnai1/Fn1/Gngt2/Pik3r6/Rasgrp2/Trpc6/Maged2/Islr/Gng11/Dgkb/Vegfc/Pecam1/Igf2/Gng2/Pros1/Arrb1/Sccpdh/Arrb2/Fyn/Tor4a/Habp4/Gnb5/Fam3c/Selenop/Gnb4/Apbb1ip/Lat/Lcp2/Lhfpl2/F2r/Plek</t>
         </is>
       </c>
+      <c r="H17">
+        <v>35</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18">
-        <v>13</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>GABA receptor activation</t>
+        </is>
       </c>
       <c r="B18">
         <v>0.2321428571428572</v>
@@ -908,18 +910,18 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>GABA receptor activation</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
           <t>Kcnj3/Gnai1/Adcy3/Gngt2/Adcy4/Adcy7/Gabra4/Gng11/Gng2/Gnb5/Arhgef9/Gnb4/Gabbr1</t>
         </is>
       </c>
+      <c r="H18">
+        <v>13</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19">
-        <v>9</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>G-protein beta:gamma signalling</t>
+        </is>
       </c>
       <c r="B19">
         <v>0.3</v>
@@ -938,18 +940,18 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>G-protein beta:gamma signalling</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
           <t>Gngt2/Pik3r6/Plcb1/Gng11/Gng2/Plcb2/Akt3/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H19">
+        <v>9</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20">
-        <v>18</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Potassium Channels</t>
+        </is>
       </c>
       <c r="B20">
         <v>0.1875</v>
@@ -968,18 +970,19 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Potassium Channels</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
           <t>Kcnk3/Kcnb2/Kcnj3/Kcna6/Kcnd2/Kcnd3/Kcnq5/Gngt2/Gng11/Kcnma1/Gng2/Kcnc4/Kcng4/Gnb5/Gnb4/Gabbr1/Kcnq4/Kcnh1</t>
         </is>
       </c>
+      <c r="H20">
+        <v>18</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21">
-        <v>7</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Generation of second messenger
+molecules</t>
+        </is>
       </c>
       <c r="B21">
         <v>0.3684210526315789</v>
@@ -998,19 +1001,19 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Generation of second messenger
-molecules</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
           <t>Itk/Cd3g/Zap70/Lat/Lcp2/Grap2/Cd4</t>
         </is>
       </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22">
-        <v>7</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>G beta:gamma signalling through PLC
+beta</t>
+        </is>
       </c>
       <c r="B22">
         <v>0.3684210526315789</v>
@@ -1029,19 +1032,18 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>G beta:gamma signalling through PLC
-beta</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
           <t>Gngt2/Plcb1/Gng11/Gng2/Plcb2/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H22">
+        <v>7</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23">
-        <v>15</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Collagen formation</t>
+        </is>
       </c>
       <c r="B23">
         <v>0.2054794520547945</v>
@@ -1060,18 +1062,19 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Collagen formation</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
           <t>Col11a1/Col26a1/P3h3/Col14a1/Col4a6/Col16a1/Col13a1/Loxl3/Col5a2/Col15a1/P3h1/Crtap/Col23a1/Col18a1/Col4a5</t>
         </is>
       </c>
+      <c r="H23">
+        <v>15</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24">
-        <v>17</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Cell surface interactions at the
+vascular wall</t>
+        </is>
       </c>
       <c r="B24">
         <v>0.1910112359550562</v>
@@ -1090,19 +1093,18 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Cell surface interactions at the
-vascular wall</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
           <t>Apob/Angpt1/Itga4/Cd44/Fn1/Jam3/Tek/Procr/Itgal/Esam/Sele/Pecam1/Pros1/Fyn/Cd84/Spn/Jam2</t>
         </is>
       </c>
+      <c r="H24">
+        <v>17</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25">
-        <v>5</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Laminin interactions</t>
+        </is>
       </c>
       <c r="B25">
         <v>0.5</v>
@@ -1121,18 +1123,19 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Laminin interactions</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
           <t>Col4a6/Lama4/Nid1/Nid2/Col4a5</t>
         </is>
       </c>
+      <c r="H25">
+        <v>5</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26">
-        <v>7</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Presynaptic function of Kainate
+receptors</t>
+        </is>
       </c>
       <c r="B26">
         <v>0.35</v>
@@ -1151,19 +1154,18 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Presynaptic function of Kainate
-receptors</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
           <t>Gngt2/Plcb1/Gng11/Gng2/Plcb2/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H26">
+        <v>7</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27">
-        <v>14</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Opioid Signalling</t>
+        </is>
       </c>
       <c r="B27">
         <v>0.2028985507246377</v>
@@ -1182,18 +1184,18 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Opioid Signalling</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
           <t>Gnai1/Pde1b/Adcy3/Gngt2/Plcb1/Adcy4/Adcy7/Gng11/Pde1a/Gng2/Plcb2/Gnb5/Gnb4/Prkar1b</t>
         </is>
       </c>
+      <c r="H27">
+        <v>14</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28">
-        <v>9</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Sialic acid metabolism</t>
+        </is>
       </c>
       <c r="B28">
         <v>0.2727272727272727</v>
@@ -1212,18 +1214,18 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Sialic acid metabolism</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
           <t>St6gal2/St8sia2/St8sia4/Npl/St3gal2/St6galnac4/St8sia6/St6galnac6/St3gal4</t>
         </is>
       </c>
+      <c r="H28">
+        <v>9</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29">
-        <v>9</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Collagen chain trimerization</t>
+        </is>
       </c>
       <c r="B29">
         <v>0.2571428571428571</v>
@@ -1242,18 +1244,19 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Collagen chain trimerization</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
           <t>Col11a1/Col26a1/Col14a1/Col16a1/Col13a1/Col5a2/Col15a1/Col23a1/Col18a1</t>
         </is>
       </c>
+      <c r="H29">
+        <v>9</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30">
-        <v>8</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Activation of kainate receptors
+upon glutamate binding</t>
+        </is>
       </c>
       <c r="B30">
         <v>0.2758620689655172</v>
@@ -1272,19 +1275,18 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Activation of kainate receptors
-upon glutamate binding</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
           <t>Gngt2/Plcb1/Gng11/Gng2/Plcb2/Dlg4/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H30">
+        <v>8</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31">
-        <v>10</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Ca2+ pathway</t>
+        </is>
       </c>
       <c r="B31">
         <v>0.2325581395348837</v>
@@ -1303,18 +1305,18 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Ca2+ pathway</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
           <t>Lef1/Wnt11/Gngt2/Plcb1/Gng11/Gng2/Plcb2/Fzd2/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H31">
+        <v>10</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32">
-        <v>24</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>RAC1 GTPase cycle</t>
+        </is>
       </c>
       <c r="B32">
         <v>0.1481481481481481</v>
@@ -1333,18 +1335,18 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>RAC1 GTPase cycle</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
           <t>Nhs/Mcam/Fermt2/Wasf3/Arhgap45/Arhgef25/Arhgap25/Dock2/Dock10/Abi2/Sh3bp1/Arhgef15/Nckap1l/Arap3/Prex2/Arhgap10/Dlc1/Arhgap31/Ngef/Fgd5/Arhgap15/Cav1/Cyfip2/Pld2</t>
         </is>
       </c>
+      <c r="H32">
+        <v>24</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33">
-        <v>47</v>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>RHO GTPase cycle</t>
+        </is>
       </c>
       <c r="B33">
         <v>0.1198979591836735</v>
@@ -1363,18 +1365,18 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>RHO GTPase cycle</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
           <t>Nhs/Mcam/Plxnb1/Ccdc88a/Pcdh7/Fermt2/Wasf3/Arhgap45/Arhgef25/Akap12/Arhgap25/Dock2/Slitrk3/Myo9a/Plxnd1/Dock10/Abi2/Sh3bp1/Arhgap6/Arhgef15/Nckap1l/Arap3/Prex2/Arhgap10/Dlc1/Arhgef26/Arhgap28/Net1/Pde5a/Fgd1/Dlg5/Arhgap31/Arfgap3/Zap70/Cep97/Ngef/Arhgef9/Fgd5/Arhgap15/Elmo2/Cav1/Cyfip2/Pld2/Wdr6/Fmnl3/Fgd2/Plekhg5</t>
         </is>
       </c>
+      <c r="H33">
+        <v>47</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34">
-        <v>19</v>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Glycosaminoglycan metabolism</t>
+        </is>
       </c>
       <c r="B34">
         <v>0.1623931623931624</v>
@@ -1393,18 +1395,18 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Glycosaminoglycan metabolism</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
           <t>Gpc6/Chst2/Cd44/Cspg4/Gpc3/B4galt2/Has2/St3gal2/Chst1/Glb1l/Bgn/Dse/Xylt1/St3gal4/Arsb/Abcc5/Gpc2/Lum/Papss2</t>
         </is>
       </c>
+      <c r="H34">
+        <v>19</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35">
-        <v>15</v>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>CDC42 GTPase cycle</t>
+        </is>
       </c>
       <c r="B35">
         <v>0.1807228915662651</v>
@@ -1423,18 +1425,19 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>CDC42 GTPase cycle</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
           <t>Arhgap45/Arhgef25/Dock10/Arhgef15/Arap3/Prex2/Arhgap10/Dlc1/Arhgef26/Fgd1/Arhgap31/Ngef/Arhgef9/Cav1/Fgd2</t>
         </is>
       </c>
+      <c r="H35">
+        <v>15</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36">
-        <v>7</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>G beta:gamma signalling through
+PI3Kgamma</t>
+        </is>
       </c>
       <c r="B36">
         <v>0.2916666666666667</v>
@@ -1453,19 +1456,19 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>G beta:gamma signalling through
-PI3Kgamma</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
           <t>Gngt2/Pik3r6/Gng11/Gng2/Akt3/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H36">
+        <v>7</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37">
-        <v>8</v>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Thrombin signalling through
+proteinase activated receptors (PARs)</t>
+        </is>
       </c>
       <c r="B37">
         <v>0.2580645161290323</v>
@@ -1484,14 +1487,11 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Thrombin signalling through
-proteinase activated receptors (PARs)</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
           <t>Gngt2/Gng11/Gng2/Arrb1/Arrb2/Gnb5/Gnb4/F2r</t>
         </is>
+      </c>
+      <c r="H37">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1510,48 +1510,50 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>GeneRatio</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pvalue</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>p.adjust</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>logFDR</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>qvalue</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>geneID</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Count</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GeneRatio</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>pvalue</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>p.adjust</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>logFDR</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>qvalue</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>geneID</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>52</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Neuronal System</t>
+        </is>
       </c>
       <c r="B2">
         <v>0.161993769470405</v>
@@ -1570,18 +1572,18 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Neuronal System</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
           <t>Kcnk3/Kcnb2/Syn2/Kcnj3/Slc1a3/Gria4/Kcna6/Kcnd2/Ptprd/Kcnd3/Nlgn1/Epb41l3/Lrrc7/Abat/Gnai1/Lrrc4b/Kcnq5/Grin2b/Adcy3/Maoa/Shank2/Gngt2/Ppfia2/Plcb1/Slitrk3/Rps6ka2/Glrb/Gabra4/Dlg2/Adcy4/Ppfia4/Gng11/Nlgn3/Lin7a/Adcy7/Tspan7/Kcnma1/Kcnc4/Gjc1/Gng2/Plcb2/Lrfn2/Kcng4/Slc38a1/Dlg4/Gnb5/Arhgef9/Gnb4/Kcnq4/Gabbr1/Cacna1a/Cacnb4</t>
         </is>
       </c>
+      <c r="H2">
+        <v>52</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>38</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Extracellular matrix organization</t>
+        </is>
       </c>
       <c r="B3">
         <v>0.1645021645021645</v>
@@ -1600,18 +1602,19 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Extracellular matrix organization</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
           <t>Col11a1/Mmp16/Col26a1/Itga4/P3h3/Col14a1/Capn6/Col4a6/Ddr2/Cd44/Lama4/Itgb7/Fn1/Mmp2/Col16a1/Icam1/Nid1/Jam3/Itga1/Col13a1/Loxl3/Itgal/Emilin1/Pecam1/Col5a2/Col15a1/Ltbp3/Mmp19/Bgn/P3h1/Adam19/Crtap/Efemp2/Col23a1/Col18a1/Itga8/Tmprss6/Itgb4</t>
         </is>
       </c>
+      <c r="H3">
+        <v>38</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4">
-        <v>12</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>O-glycosylation of TSR
+domain-containing proteins</t>
+        </is>
       </c>
       <c r="B4">
         <v>0.3636363636363636</v>
@@ -1630,19 +1633,19 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>O-glycosylation of TSR
-domain-containing proteins</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
           <t>Adamts20/Sema5b/Adamts16/Adamts19/Thsd7b/Thsd1/Adamts1/Adamts10/Adamts7/Adamtsl1/Sbspon/Adamts17</t>
         </is>
       </c>
+      <c r="H4">
+        <v>12</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5">
-        <v>33</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Transmission across Chemical
+Synapses</t>
+        </is>
       </c>
       <c r="B5">
         <v>0.1658291457286432</v>
@@ -1661,19 +1664,18 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Transmission across Chemical
-Synapses</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
           <t>Syn2/Kcnj3/Slc1a3/Gria4/Lrrc7/Abat/Gnai1/Grin2b/Adcy3/Maoa/Gngt2/Ppfia2/Plcb1/Rps6ka2/Glrb/Gabra4/Dlg2/Adcy4/Ppfia4/Gng11/Lin7a/Adcy7/Tspan7/Gng2/Plcb2/Slc38a1/Dlg4/Gnb5/Arhgef9/Gnb4/Gabbr1/Cacna1a/Cacnb4</t>
         </is>
       </c>
+      <c r="H5">
+        <v>33</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6">
-        <v>60</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Hemostasis</t>
+        </is>
       </c>
       <c r="B6">
         <v>0.1226993865030675</v>
@@ -1692,18 +1694,18 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Hemostasis</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
           <t>Apob/Hgf/Angpt1/Itga4/Cd109/Igf1/Tfpi/Nos3/Slc8a1/Cd44/Pcdh7/P2rx2/Gnai1/Fn1/Serpine2/Tek/Pde1b/Jam3/Gngt2/Pik3r6/Slc8a3/Rasgrp2/Dock2/Sh2b2/Kif26a/Dock10/Trpc6/Procr/Gng11/Islr/Esam/Itgal/Dgkb/Vegfc/Tubb4a/Pde1a/Maged2/Sele/Kif6/Igf2/Pecam1/Pros1/Gng2/Arrb1/Sccpdh/Pde5a/Cd84/Arrb2/Fyn/Fgr/Atp2b4/Tor4a/Selenop/Gnb5/Lat/Fam3c/Habp4/Apbb1ip/Gnb4/Kif16b</t>
         </is>
       </c>
+      <c r="H6">
+        <v>60</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7">
-        <v>17</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Platelet homeostasis</t>
+        </is>
       </c>
       <c r="B7">
         <v>0.2394366197183098</v>
@@ -1722,18 +1724,18 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Platelet homeostasis</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
           <t>Apob/Nos3/Slc8a1/P2rx2/Pde1b/Gngt2/Slc8a3/Trpc6/Gng11/Pde1a/Pecam1/Gng2/Pde5a/Fgr/Atp2b4/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H7">
+        <v>17</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8">
-        <v>19</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>O-linked glycosylation</t>
+        </is>
       </c>
       <c r="B8">
         <v>0.1979166666666667</v>
@@ -1752,18 +1754,18 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>O-linked glycosylation</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
           <t>Adamts20/Sema5b/Adamts16/Adamts19/Thsd7b/Thsd1/Adamts1/Galnt16/St6galnac4/St3gal2/Adamts10/Adamts7/Galntl6/Adamtsl1/B3gnt5/Sbspon/St3gal4/Large1/Adamts17</t>
         </is>
       </c>
+      <c r="H8">
+        <v>19</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9">
-        <v>10</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>G alpha (z) signalling events</t>
+        </is>
       </c>
       <c r="B9">
         <v>0.3225806451612903</v>
@@ -1782,18 +1784,18 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>G alpha (z) signalling events</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
           <t>Rgs16/Adcy3/Gngt2/Adcy4/Gng11/Adcy7/Gng2/Gnaz/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10">
-        <v>15</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Integrin cell surface interactions</t>
+        </is>
       </c>
       <c r="B10">
         <v>0.2272727272727273</v>
@@ -1812,18 +1814,19 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Integrin cell surface interactions</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
           <t>Itga4/Col4a6/Cd44/Itgb7/Fn1/Col16a1/Icam1/Jam3/Itga1/Col13a1/Itgal/Pecam1/Col5a2/Col18a1/Itga8</t>
         </is>
       </c>
+      <c r="H10">
+        <v>15</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11">
-        <v>23</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Neurotransmitter receptors and
+postsynaptic signal transmission</t>
+        </is>
       </c>
       <c r="B11">
         <v>0.1691176470588235</v>
@@ -1842,19 +1845,18 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Neurotransmitter receptors and
-postsynaptic signal transmission</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
           <t>Kcnj3/Gria4/Lrrc7/Gnai1/Grin2b/Adcy3/Gngt2/Plcb1/Rps6ka2/Glrb/Gabra4/Dlg2/Adcy4/Gng11/Adcy7/Tspan7/Gng2/Plcb2/Dlg4/Gnb5/Arhgef9/Gnb4/Gabbr1</t>
         </is>
       </c>
+      <c r="H11">
+        <v>23</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12">
-        <v>11</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>GABA B receptor activation</t>
+        </is>
       </c>
       <c r="B12">
         <v>0.275</v>
@@ -1873,18 +1875,18 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>GABA B receptor activation</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
           <t>Kcnj3/Gnai1/Adcy3/Gngt2/Adcy4/Gng11/Adcy7/Gng2/Gnb5/Gnb4/Gabbr1</t>
         </is>
       </c>
+      <c r="H12">
+        <v>11</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13">
-        <v>11</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Activation of GABAB receptors</t>
+        </is>
       </c>
       <c r="B13">
         <v>0.275</v>
@@ -1903,18 +1905,18 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Activation of GABAB receptors</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
           <t>Kcnj3/Gnai1/Adcy3/Gngt2/Adcy4/Gng11/Adcy7/Gng2/Gnb5/Gnb4/Gabbr1</t>
         </is>
       </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14">
-        <v>13</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>GABA receptor activation</t>
+        </is>
       </c>
       <c r="B14">
         <v>0.2321428571428572</v>
@@ -1933,18 +1935,19 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>GABA receptor activation</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
           <t>Kcnj3/Gnai1/Adcy3/Gngt2/Gabra4/Adcy4/Gng11/Adcy7/Gng2/Gnb5/Arhgef9/Gnb4/Gabbr1</t>
         </is>
       </c>
+      <c r="H14">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15">
-        <v>14</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Protein-protein interactions at
+synapses</t>
+        </is>
       </c>
       <c r="B15">
         <v>0.2121212121212121</v>
@@ -1963,19 +1966,18 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Protein-protein interactions at
-synapses</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
           <t>Gria4/Ptprd/Nlgn1/Epb41l3/Lrrc4b/Grin2b/Shank2/Ppfia2/Slitrk3/Dlg2/Ppfia4/Nlgn3/Lrfn2/Dlg4</t>
         </is>
       </c>
+      <c r="H15">
+        <v>14</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16">
-        <v>9</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>G-protein beta:gamma signalling</t>
+        </is>
       </c>
       <c r="B16">
         <v>0.3</v>
@@ -1994,18 +1996,19 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>G-protein beta:gamma signalling</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
           <t>Gngt2/Pik3r6/Plcb1/Gng11/Gng2/Plcb2/Akt3/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H16">
+        <v>9</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17">
-        <v>13</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Collagen biosynthesis and modifying
+enzymes</t>
+        </is>
       </c>
       <c r="B17">
         <v>0.2166666666666667</v>
@@ -2024,19 +2027,19 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Collagen biosynthesis and modifying
-enzymes</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
           <t>Col11a1/Col26a1/P3h3/Col14a1/Col4a6/Col16a1/Col13a1/Col5a2/Col15a1/P3h1/Crtap/Col23a1/Col18a1</t>
         </is>
       </c>
+      <c r="H17">
+        <v>13</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18">
-        <v>7</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>G beta:gamma signalling through PLC
+beta</t>
+        </is>
       </c>
       <c r="B18">
         <v>0.3684210526315789</v>
@@ -2055,19 +2058,18 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>G beta:gamma signalling through PLC
-beta</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
           <t>Gngt2/Plcb1/Gng11/Gng2/Plcb2/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H18">
+        <v>7</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19">
-        <v>14</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>G alpha (12/13) signalling events</t>
+        </is>
       </c>
       <c r="B19">
         <v>0.2</v>
@@ -2086,18 +2088,18 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>G alpha (12/13) signalling events</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
           <t>Plxnb1/Adra1a/Arhgef25/Gngt2/Gng11/Arhgef15/Gng2/Arhgef26/Net1/Fgd1/Gnb5/Ngef/Arhgef9/Gnb4</t>
         </is>
       </c>
+      <c r="H19">
+        <v>14</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20">
-        <v>17</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Potassium Channels</t>
+        </is>
       </c>
       <c r="B20">
         <v>0.1770833333333333</v>
@@ -2116,18 +2118,19 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Potassium Channels</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
           <t>Kcnk3/Kcnb2/Kcnj3/Kcna6/Kcnd2/Kcnd3/Kcnq5/Gngt2/Gng11/Kcnma1/Kcnc4/Gng2/Kcng4/Gnb5/Gnb4/Kcnq4/Gabbr1</t>
         </is>
       </c>
+      <c r="H20">
+        <v>17</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21">
-        <v>7</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Presynaptic function of Kainate
+receptors</t>
+        </is>
       </c>
       <c r="B21">
         <v>0.35</v>
@@ -2146,19 +2149,18 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Presynaptic function of Kainate
-receptors</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
           <t>Gngt2/Plcb1/Gng11/Gng2/Plcb2/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22">
-        <v>9</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Sialic acid metabolism</t>
+        </is>
       </c>
       <c r="B22">
         <v>0.2727272727272727</v>
@@ -2177,18 +2179,18 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Sialic acid metabolism</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
           <t>St6gal2/St8sia2/St8sia4/Npl/St6galnac4/St3gal2/St8sia6/St6galnac6/St3gal4</t>
         </is>
       </c>
+      <c r="H22">
+        <v>9</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23">
-        <v>14</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Collagen formation</t>
+        </is>
       </c>
       <c r="B23">
         <v>0.1917808219178082</v>
@@ -2207,18 +2209,19 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Collagen formation</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
           <t>Col11a1/Col26a1/P3h3/Col14a1/Col4a6/Col16a1/Col13a1/Loxl3/Col5a2/Col15a1/P3h1/Crtap/Col23a1/Col18a1</t>
         </is>
       </c>
+      <c r="H23">
+        <v>14</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24">
-        <v>31</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Platelet activation, signaling and
+aggregation</t>
+        </is>
       </c>
       <c r="B24">
         <v>0.1275720164609054</v>
@@ -2237,19 +2240,18 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Platelet activation, signaling and
-aggregation</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
           <t>Hgf/Cd109/Igf1/Pcdh7/Gnai1/Fn1/Gngt2/Pik3r6/Rasgrp2/Trpc6/Gng11/Islr/Dgkb/Vegfc/Maged2/Igf2/Pecam1/Pros1/Gng2/Arrb1/Sccpdh/Arrb2/Fyn/Tor4a/Selenop/Gnb5/Lat/Fam3c/Habp4/Apbb1ip/Gnb4</t>
         </is>
       </c>
+      <c r="H24">
+        <v>31</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25">
-        <v>9</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Collagen chain trimerization</t>
+        </is>
       </c>
       <c r="B25">
         <v>0.2571428571428571</v>
@@ -2268,18 +2270,18 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Collagen chain trimerization</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
           <t>Col11a1/Col26a1/Col14a1/Col16a1/Col13a1/Col5a2/Col15a1/Col23a1/Col18a1</t>
         </is>
       </c>
+      <c r="H25">
+        <v>9</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26">
-        <v>10</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Ca2+ pathway</t>
+        </is>
       </c>
       <c r="B26">
         <v>0.2325581395348837</v>
@@ -2298,18 +2300,18 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Ca2+ pathway</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
           <t>Lef1/Wnt11/Gngt2/Plcb1/Gng11/Gng2/Plcb2/Fzd2/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27">
-        <v>23</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>RAC1 GTPase cycle</t>
+        </is>
       </c>
       <c r="B27">
         <v>0.1419753086419753</v>
@@ -2328,18 +2330,19 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>RAC1 GTPase cycle</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
           <t>Nhs/Mcam/Fermt2/Wasf3/Arhgap45/Arhgef25/Arhgap25/Dock2/Dock10/Abi2/Sh3bp1/Arhgef15/Nckap1l/Arap3/Prex2/Arhgap10/Dlc1/Arhgap31/Ngef/Fgd5/Arhgap15/Cav1/Cyfip2</t>
         </is>
       </c>
+      <c r="H27">
+        <v>23</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28">
-        <v>8</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Activation of kainate receptors
+upon glutamate binding</t>
+        </is>
       </c>
       <c r="B28">
         <v>0.2758620689655172</v>
@@ -2358,19 +2361,18 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Activation of kainate receptors
-upon glutamate binding</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
           <t>Gngt2/Plcb1/Gng11/Gng2/Plcb2/Dlg4/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H28">
+        <v>8</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29">
-        <v>13</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Opioid Signalling</t>
+        </is>
       </c>
       <c r="B29">
         <v>0.1884057971014493</v>
@@ -2389,18 +2391,19 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Opioid Signalling</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
           <t>Gnai1/Pde1b/Adcy3/Gngt2/Plcb1/Adcy4/Gng11/Adcy7/Pde1a/Gng2/Plcb2/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H29">
+        <v>13</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30">
-        <v>7</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>G beta:gamma signalling through
+PI3Kgamma</t>
+        </is>
       </c>
       <c r="B30">
         <v>0.2916666666666667</v>
@@ -2419,19 +2422,19 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>G beta:gamma signalling through
-PI3Kgamma</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
           <t>Gngt2/Pik3r6/Gng11/Gng2/Akt3/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H30">
+        <v>7</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31">
-        <v>15</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Cell surface interactions at the
+vascular wall</t>
+        </is>
       </c>
       <c r="B31">
         <v>0.1685393258426966</v>
@@ -2450,19 +2453,18 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Cell surface interactions at the
-vascular wall</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
           <t>Apob/Angpt1/Itga4/Cd44/Fn1/Tek/Jam3/Procr/Esam/Itgal/Sele/Pecam1/Pros1/Cd84/Fyn</t>
         </is>
       </c>
+      <c r="H31">
+        <v>15</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32">
-        <v>12</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Cell junction organization</t>
+        </is>
       </c>
       <c r="B32">
         <v>0.1875</v>
@@ -2481,18 +2483,18 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Cell junction organization</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
           <t>Sdk2/Fermt2/Cdh2/Cdh6/Cdh13/Cdh10/Cdh5/Cdh11/Pard6g/Parvb/Flnc/Itgb4</t>
         </is>
       </c>
+      <c r="H32">
+        <v>12</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33">
-        <v>14</v>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CDC42 GTPase cycle</t>
+        </is>
       </c>
       <c r="B33">
         <v>0.1686746987951807</v>
@@ -2511,18 +2513,18 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>CDC42 GTPase cycle</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
           <t>Arhgap45/Arhgef25/Dock10/Arhgef15/Arap3/Prex2/Arhgef26/Arhgap10/Dlc1/Fgd1/Arhgap31/Ngef/Arhgef9/Cav1</t>
         </is>
       </c>
+      <c r="H33">
+        <v>14</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34">
-        <v>21</v>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Muscle contraction</t>
+        </is>
       </c>
       <c r="B34">
         <v>0.1372549019607843</v>
@@ -2541,18 +2543,19 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Muscle contraction</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
           <t>Kcnk3/Cacna1c/Kcnd2/Ryr1/Kcnd3/Slc8a1/Tmod2/Gucy1a2/Slc8a3/Itga1/Gucy1b1/Mme/Gucy1a1/Myl3/Cacng7/Kcnip3/Asph/Ryr3/Pde5a/Atp2b4/Atp1a2</t>
         </is>
       </c>
+      <c r="H34">
+        <v>21</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35">
-        <v>7</v>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Activation of G protein gated
+Potassium channels</t>
+        </is>
       </c>
       <c r="B35">
         <v>0.2592592592592592</v>
@@ -2571,19 +2574,18 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Activation of G protein gated
-Potassium channels</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
           <t>Kcnj3/Gngt2/Gng11/Gng2/Gnb5/Gnb4/Gabbr1</t>
         </is>
       </c>
+      <c r="H35">
+        <v>7</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36">
-        <v>7</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>G protein gated Potassium channels</t>
+        </is>
       </c>
       <c r="B36">
         <v>0.2592592592592592</v>
@@ -2602,18 +2604,19 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>G protein gated Potassium channels</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
           <t>Kcnj3/Gngt2/Gng11/Gng2/Gnb5/Gnb4/Gabbr1</t>
         </is>
       </c>
+      <c r="H36">
+        <v>7</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37">
-        <v>7</v>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Inhibition  of voltage gated Ca2+
+channels via Gbeta/gamma subunits</t>
+        </is>
       </c>
       <c r="B37">
         <v>0.2592592592592592</v>
@@ -2632,19 +2635,18 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Inhibition  of voltage gated Ca2+
-channels via Gbeta/gamma subunits</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
           <t>Kcnj3/Gngt2/Gng11/Gng2/Gnb5/Gnb4/Gabbr1</t>
         </is>
       </c>
+      <c r="H37">
+        <v>7</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38">
-        <v>17</v>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Glycosaminoglycan metabolism</t>
+        </is>
       </c>
       <c r="B38">
         <v>0.1452991452991453</v>
@@ -2663,18 +2665,19 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Glycosaminoglycan metabolism</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
           <t>Gpc6/Chst2/Cd44/Cspg4/Gpc3/B4galt2/Has2/St3gal2/Chst1/Glb1l/Bgn/Xylt1/Dse/St3gal4/Arsb/Gpc2/Abcc5</t>
         </is>
       </c>
+      <c r="H38">
+        <v>17</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39">
-        <v>6</v>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>ADP signalling through P2Y
+purinoceptor 12</t>
+        </is>
       </c>
       <c r="B39">
         <v>0.2857142857142857</v>
@@ -2693,19 +2696,19 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>ADP signalling through P2Y
-purinoceptor 12</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
           <t>Gnai1/Gngt2/Gng11/Gng2/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H39">
+        <v>6</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40">
-        <v>6</v>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Adrenaline,noradrenaline inhibits
+insulin secretion</t>
+        </is>
       </c>
       <c r="B40">
         <v>0.2727272727272727</v>
@@ -2724,19 +2727,18 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Adrenaline,noradrenaline inhibits
-insulin secretion</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
           <t>Gnai1/Gngt2/Gng11/Gng2/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H40">
+        <v>6</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41">
-        <v>41</v>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>RHO GTPase cycle</t>
+        </is>
       </c>
       <c r="B41">
         <v>0.1045918367346939</v>
@@ -2755,18 +2757,18 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>RHO GTPase cycle</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
           <t>Nhs/Mcam/Plxnb1/Ccdc88a/Pcdh7/Fermt2/Wasf3/Arhgap45/Arhgef25/Akap12/Arhgap25/Dock2/Slitrk3/Plxnd1/Dock10/Abi2/Myo9a/Sh3bp1/Arhgef15/Arhgap6/Nckap1l/Arap3/Prex2/Arhgef26/Arhgap10/Arhgap28/Pde5a/Dlc1/Net1/Fgd1/Zap70/Dlg5/Arhgap31/Ngef/Fgd5/Arhgef9/Cep97/Arhgap15/Arfgap3/Cav1/Cyfip2</t>
         </is>
       </c>
+      <c r="H41">
+        <v>41</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42">
-        <v>24</v>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>G alpha (q) signalling events</t>
+        </is>
       </c>
       <c r="B42">
         <v>0.1218274111675127</v>
@@ -2785,18 +2787,19 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>G alpha (q) signalling events</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
           <t>Adra1a/Rgs16/Ednrb/Lpar4/Arhgef25/Gngt2/Ptgfr/Edn3/Plcb1/Rps6ka2/Trpc6/Gng11/Dgkb/Rgs5/Agtr1a/Ednra/Bdkrb2/Xcl1/Htr2a/Gng2/Plcb2/Gnb5/Prokr1/Gnb4</t>
         </is>
       </c>
+      <c r="H42">
+        <v>24</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43">
-        <v>10</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Class B/2 (Secretin family
+receptors)</t>
+        </is>
       </c>
       <c r="B43">
         <v>0.1818181818181818</v>
@@ -2815,19 +2818,18 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Class B/2 (Secretin family
-receptors)</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
           <t>Vipr2/Gngt2/Calca/Pth1r/Gng11/Adcyap1r1/Gng2/Calcrl/Gnb5/Gnb4</t>
         </is>
       </c>
+      <c r="H43">
+        <v>10</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44">
-        <v>13</v>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Cell-Cell communication</t>
+        </is>
       </c>
       <c r="B44">
         <v>0.1566265060240964</v>
@@ -2846,18 +2848,19 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Cell-Cell communication</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
           <t>Sdk2/Fermt2/Cdh2/Cdh6/Cdh13/Cdh10/Cdh5/Cdh11/Pard6g/Parvb/Flnc/Fyn/Itgb4</t>
         </is>
       </c>
+      <c r="H44">
+        <v>13</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45">
-        <v>6</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>A tetrasaccharide linker sequence
+is required for GAG synthesis</t>
+        </is>
       </c>
       <c r="B45">
         <v>0.2608695652173913</v>
@@ -2876,19 +2879,19 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>A tetrasaccharide linker sequence
-is required for GAG synthesis</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
           <t>Gpc6/Cspg4/Gpc3/Bgn/Xylt1/Gpc2</t>
         </is>
       </c>
+      <c r="H45">
+        <v>6</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46">
-        <v>6</v>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>N-glycan antennae elongation in the
+medial/trans-Golgi</t>
+        </is>
       </c>
       <c r="B46">
         <v>0.2608695652173913</v>
@@ -2907,14 +2910,11 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>N-glycan antennae elongation in the
-medial/trans-Golgi</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
           <t>St8sia2/Man2a2/Chst10/B4galt2/St8sia6/St3gal4</t>
         </is>
+      </c>
+      <c r="H46">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2933,48 +2933,50 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>GeneRatio</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pvalue</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>p.adjust</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>logFDR</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>qvalue</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>geneID</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Count</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GeneRatio</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>pvalue</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>p.adjust</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>logFDR</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>qvalue</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>geneID</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>20</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Neuronal System</t>
+        </is>
       </c>
       <c r="B2">
         <v>0.06230529595015576</v>
@@ -2993,18 +2995,19 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Neuronal System</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
           <t>Kcnk3/Kcnb2/Syn2/Kcnj3/Slc1a3/Kcnd2/Gria4/Kcna6/Kcnd3/Lrrc7/Nlgn1/Ptprd/Abat/Epb41l3/Lrrc4b/Gnai1/Kcnq5/Ppfia2/Grin2b/Gabra4</t>
         </is>
       </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>7</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Protein-protein interactions at
+synapses</t>
+        </is>
       </c>
       <c r="B3">
         <v>0.1060606060606061</v>
@@ -3023,19 +3026,19 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Protein-protein interactions at
-synapses</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
           <t>Gria4/Nlgn1/Ptprd/Epb41l3/Lrrc4b/Ppfia2/Grin2b</t>
         </is>
       </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4">
-        <v>5</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>O-glycosylation of TSR
+domain-containing proteins</t>
+        </is>
       </c>
       <c r="B4">
         <v>0.1515151515151515</v>
@@ -3054,19 +3057,18 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>O-glycosylation of TSR
-domain-containing proteins</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
           <t>Adamts20/Sema5b/Adamts16/Thsd7b/Adamts19</t>
         </is>
       </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5">
-        <v>13</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Axon guidance</t>
+        </is>
       </c>
       <c r="B5">
         <v>0.05220883534136546</v>
@@ -3085,18 +3087,18 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Axon guidance</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
           <t>Gap43/Epha8/Efnb3/Dcc/St8sia2/Plxnb1/St8sia4/Dab1/Evl/Grin2b/Sema7a/Mmp2/Cxcl12</t>
         </is>
       </c>
+      <c r="H5">
+        <v>13</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6">
-        <v>13</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Nervous system development</t>
+        </is>
       </c>
       <c r="B6">
         <v>0.052</v>
@@ -3115,18 +3117,19 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Nervous system development</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
           <t>Gap43/Epha8/Efnb3/Dcc/St8sia2/Plxnb1/St8sia4/Dab1/Evl/Grin2b/Sema7a/Mmp2/Cxcl12</t>
         </is>
       </c>
+      <c r="H6">
+        <v>13</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7">
-        <v>8</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Degradation of the extracellular
+matrix</t>
+        </is>
       </c>
       <c r="B7">
         <v>0.07476635514018691</v>
@@ -3145,19 +3148,18 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Degradation of the extracellular
-matrix</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
           <t>Col11a1/Mmp16/Col26a1/Capn6/Col4a6/Cd44/Mmp2/Nid1</t>
         </is>
       </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8">
-        <v>3</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Laminin interactions</t>
+        </is>
       </c>
       <c r="B8">
         <v>0.3</v>
@@ -3176,18 +3178,18 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Laminin interactions</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
           <t>Col4a6/Lama4/Nid1</t>
         </is>
       </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9">
-        <v>5</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Voltage gated Potassium channels</t>
+        </is>
       </c>
       <c r="B9">
         <v>0.125</v>
@@ -3206,18 +3208,18 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Voltage gated Potassium channels</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
           <t>Kcnb2/Kcnd2/Kcna6/Kcnd3/Kcnq5</t>
         </is>
       </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10">
-        <v>12</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Extracellular matrix organization</t>
+        </is>
       </c>
       <c r="B10">
         <v>0.05194805194805195</v>
@@ -3236,18 +3238,18 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Extracellular matrix organization</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
           <t>Col11a1/Mmp16/Col26a1/Col14a1/Capn6/Col4a6/Itga4/P3h3/Cd44/Mmp2/Lama4/Nid1</t>
         </is>
       </c>
+      <c r="H10">
+        <v>12</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11">
-        <v>5</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Retinoid metabolism and transport</t>
+        </is>
       </c>
       <c r="B11">
         <v>0.119047619047619</v>
@@ -3266,18 +3268,18 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Retinoid metabolism and transport</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
           <t>Gpc6/Apob/Ttr/Gpc3/Lrp2</t>
         </is>
       </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12">
-        <v>5</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Metabolism of fat-soluble vitamins</t>
+        </is>
       </c>
       <c r="B12">
         <v>0.108695652173913</v>
@@ -3296,18 +3298,18 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Metabolism of fat-soluble vitamins</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
           <t>Gpc6/Apob/Ttr/Gpc3/Lrp2</t>
         </is>
       </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13">
-        <v>7</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Potassium Channels</t>
+        </is>
       </c>
       <c r="B13">
         <v>0.07291666666666667</v>
@@ -3326,13 +3328,11 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Potassium Channels</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
           <t>Kcnk3/Kcnb2/Kcnj3/Kcnd2/Kcna6/Kcnd3/Kcnq5</t>
         </is>
+      </c>
+      <c r="H13">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>